<commit_message>
bios and event format
</commit_message>
<xml_diff>
--- a/static/data/members.xlsx
+++ b/static/data/members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\PersonalProjects\SVG_site\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5029D325-DEA8-4AA6-92B6-66702035501D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1087371F-1616-4B37-A6C5-F8953588D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Murphy</t>
   </si>
   <si>
-    <t>Gracie is an MIMG major with a minor in Professional Writing. She has been working with the Jacobs Laboratory for the past year researching the impact of the human gut microbiome on stress and human disease. She loves working with kids and is excited to work with local elementary and middle schools this upcoming year.</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -183,7 +180,10 @@
     <t>Art and Web Design</t>
   </si>
   <si>
-    <t>Hi, I'm Tyler! I'm a fourth year data theory and cognitive science major. In my free time I enjoy, drawing, coding, and plyaing basketball. I'm always interested in learning more about a variety of subjects, including biology. Thus, I hope this year I can learn more about virology, while contributing to the creative side of this organization.</t>
+    <t>I am currently a 3rd year an MIMG major with a minor in Professional Writing. I have been working with the Jacob’s Laboratory for the past year researching the impact of the human gut microbiome on stress and human disease. I love working with kids and am excited to work with local elementary and middle schools this upcoming year.</t>
+  </si>
+  <si>
+    <t>Hey y'all. I'm a fourth year data theory and cognitive science major. In my free time I enjoy, drawing, coding, and plyaing basketball. I'm always interested in learning more about a variety of subjects, including biology. Thus, I hope this year I can learn more about virology, while contributing to the creative side of this organization.</t>
   </si>
 </sst>
 </file>
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -569,10 +569,10 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -586,7 +586,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -595,10 +595,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -612,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>16</v>
@@ -638,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
@@ -647,7 +647,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>19</v>
@@ -664,7 +664,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -684,25 +684,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -710,25 +710,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -736,22 +736,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>52</v>

</xml_diff>